<commit_message>
Add the picture of small squares, making small additions to forms
</commit_message>
<xml_diff>
--- a/To do list.xlsx
+++ b/To do list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Завдання</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>підтримка бд</t>
+  </si>
+  <si>
+    <t>Оля</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>Коментарі</t>
+  </si>
+  <si>
+    <t>Трабл з підключенням файлів ресурсів</t>
   </si>
 </sst>
 </file>
@@ -92,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +184,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -446,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,9 +478,10 @@
     <col min="2" max="2" width="25" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="19.88671875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="54" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,43 +494,55 @@
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="E1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>